<commit_message>
plot of distribution: downloads--> usage
</commit_message>
<xml_diff>
--- a/data/results/high_rank_value.xlsx
+++ b/data/results/high_rank_value.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="3030" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="genbank" sheetId="1" r:id="rId1"/>
@@ -225,10 +225,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DEFINITION</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Using AmgX to Accelerate PETSc-Based CFD Codes</t>
   </si>
   <si>
@@ -291,6 +287,10 @@
   </si>
   <si>
     <t xml:space="preserve">year </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEFINITION</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -648,15 +648,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="11.625" style="1" customWidth="1"/>
     <col min="3" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="18.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="255.625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
@@ -664,7 +664,7 @@
         <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1027,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1043,7 +1043,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -1086,7 +1086,7 @@
         <v>1.37713900537929</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1103,7 +1103,7 @@
         <v>1.375</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1120,7 +1120,7 @@
         <v>1.32622942450071</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1137,7 +1137,7 @@
         <v>1.1875</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -1154,7 +1154,7 @@
         <v>1.1875</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -1171,7 +1171,7 @@
         <v>1.1875</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1188,7 +1188,7 @@
         <v>1.13872942450071</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1205,7 +1205,7 @@
         <v>1.13872942450071</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1222,7 +1222,7 @@
         <v>1.13872942450071</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -1239,7 +1239,7 @@
         <v>1.13872942450071</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -1256,7 +1256,7 @@
         <v>1.1366175573036299</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -1273,7 +1273,7 @@
         <v>1.1318917358318401</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -1290,7 +1290,7 @@
         <v>1.1245674800110199</v>
       </c>
       <c r="E15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -1307,7 +1307,7 @@
         <v>1.11217668001322</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -1324,7 +1324,7 @@
         <v>1.11217668001322</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -1341,7 +1341,7 @@
         <v>1.09375</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -1358,7 +1358,7 @@
         <v>1.09375</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -1375,7 +1375,7 @@
         <v>1.08918421494</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -1392,7 +1392,7 @@
         <v>1.0833333333333299</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>